<commit_message>
Updated tables and completed document references
</commit_message>
<xml_diff>
--- a/Docs/tabels.xlsx
+++ b/Docs/tabels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\Técnico\CRC\Projeto\Workspace\CRC2021\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1CF011-A948-43FC-98A4-A07B427C93DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3830D297-CCC0-44F1-BD3D-1AB472E4E784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Network</t>
   </si>
@@ -97,12 +97,36 @@
   </si>
   <si>
     <t>Modularity</t>
+  </si>
+  <si>
+    <t>~0</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>ACS - Average Community Size</t>
+  </si>
+  <si>
+    <t>APL - Communities Average Path Length</t>
+  </si>
+  <si>
+    <t>AID - Average Internal Degree</t>
+  </si>
+  <si>
+    <t>AE - Average Embeddedness</t>
+  </si>
+  <si>
+    <t>AT - Average Transitivity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,9 +275,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -287,12 +310,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
+  <dxfs count="44">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -308,40 +345,43 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -390,6 +430,134 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -775,7 +943,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31DF3AB8-3104-4D0E-8AD4-541FE248DB97}" name="Tabela1" displayName="Tabela1" ref="B2:H6" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31DF3AB8-3104-4D0E-8AD4-541FE248DB97}" name="Tabela1" displayName="Tabela1" ref="B2:H6" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <autoFilter ref="B2:H6" xr:uid="{31DF3AB8-3104-4D0E-8AD4-541FE248DB97}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -786,20 +954,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BD9952FD-0516-4DE7-AC4D-017A020533D1}" name="Network" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{7386C339-71D4-47E9-BB57-576DC80A209D}" name="Nodes" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{FEEA27C9-FF81-449F-9E80-3D17946AA0B9}" name="Edges" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{4EEC6697-EC02-48E8-9668-184EE35D19F6}" name="Expected Communities" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{AEE8D59E-83A0-4523-9764-B684394C284A}" name="Average Degree" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{04D4A988-05CD-4155-AC07-A21AD8D954FB}" name="Average Path Length" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{902807E3-1B6C-4D3C-8CEC-6EB17B07CB8F}" name="Clustering Coefficient" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{BD9952FD-0516-4DE7-AC4D-017A020533D1}" name="Network" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{7386C339-71D4-47E9-BB57-576DC80A209D}" name="Nodes" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{FEEA27C9-FF81-449F-9E80-3D17946AA0B9}" name="Edges" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{4EEC6697-EC02-48E8-9668-184EE35D19F6}" name="Expected Communities" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{AEE8D59E-83A0-4523-9764-B684394C284A}" name="Average Degree" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{04D4A988-05CD-4155-AC07-A21AD8D954FB}" name="Average Path Length" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{902807E3-1B6C-4D3C-8CEC-6EB17B07CB8F}" name="Clustering Coefficient" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{599D0100-3BF9-48A2-872A-937F7ACFB5B7}" name="Tabela2" displayName="Tabela2" ref="J2:P6" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{599D0100-3BF9-48A2-872A-937F7ACFB5B7}" name="Tabela2" displayName="Tabela2" ref="J2:P6" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="J2:P6" xr:uid="{599D0100-3BF9-48A2-872A-937F7ACFB5B7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -810,20 +978,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FD4ABEAB-CAAB-496C-BF1A-82EE5504C5A4}" name="Algorithm" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{1B8DE182-6929-42F3-8465-295D7488B206}" name="Communities" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{0CD33555-C038-4D78-8C24-AF1B9E679672}" name="ACS" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{FDA597C5-604A-4969-941B-602081FA8FF7}" name="APL" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{CDA6880E-F377-42F6-8BE5-76AB5FFF22C4}" name="AID" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{4F2E73CA-E516-452D-8966-7EC0060CA68C}" name="AE" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{211C7631-7466-446F-B2F3-B8B55B460F9B}" name="AT" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{FD4ABEAB-CAAB-496C-BF1A-82EE5504C5A4}" name="Algorithm" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{1B8DE182-6929-42F3-8465-295D7488B206}" name="Communities" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{0CD33555-C038-4D78-8C24-AF1B9E679672}" name="ACS" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{FDA597C5-604A-4969-941B-602081FA8FF7}" name="APL" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{CDA6880E-F377-42F6-8BE5-76AB5FFF22C4}" name="AID" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{4F2E73CA-E516-452D-8966-7EC0060CA68C}" name="AE" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{211C7631-7466-446F-B2F3-B8B55B460F9B}" name="AT" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B536BF37-0E95-45A4-B5A0-FD1E95322902}" name="Tabela3" displayName="Tabela3" ref="R2:V6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B536BF37-0E95-45A4-B5A0-FD1E95322902}" name="Tabela3" displayName="Tabela3" ref="R2:V6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="R2:V6" xr:uid="{B536BF37-0E95-45A4-B5A0-FD1E95322902}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -837,6 +1005,26 @@
     <tableColumn id="3" xr3:uid="{22B2361F-79E6-4EDC-AD51-FC1AE8CE8450}" name="Leiden" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{413FC47F-EFE5-4F44-BE40-794E7E3FB01C}" name="Girvan-Newman" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{2281036E-87EA-4797-8AFC-4FE931C35092}" name="Infomap" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECDDCFD9-1E28-4014-B9F6-17D6A219A546}" name="Tabela4" displayName="Tabela4" ref="R9:V10" totalsRowShown="0" headerRowDxfId="5" dataDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="R9:V10" xr:uid="{ECDDCFD9-1E28-4014-B9F6-17D6A219A546}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B01D6B58-CA1D-4487-B487-AEE57796A3A9}" name="Accuracy" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{3AF1ACE6-5EA7-409C-B81D-5FB98FF28A16}" name="Louvain" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{F77036A0-0023-4C76-9749-DD1A89774D0F}" name="Leiden" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{D6CDCBB9-D401-4A66-918B-2C2ADD1CB811}" name="Girvan-Newman" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{F6D701C3-4384-4C32-8828-AB99B57085FF}" name="Infomap" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1105,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:V9"/>
+  <dimension ref="B2:V12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,302 +1312,370 @@
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.77734375" customWidth="1"/>
-    <col min="19" max="19" width="9.21875" customWidth="1"/>
+    <col min="19" max="20" width="9.5546875" customWidth="1"/>
     <col min="21" max="21" width="16.109375" customWidth="1"/>
     <col min="22" max="22" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1005</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>16706</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>42</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>33</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>2.5870000000000002</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>0.39900000000000002</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>28</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>36</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>0.66900000000000004</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <v>7.141</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5">
         <v>0.90300000000000002</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <v>0.17699999999999999</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="13">
         <v>0.43099999999999999</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="13">
         <v>0.433</v>
       </c>
-      <c r="U3" s="6">
+      <c r="U3" s="13">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="14">
         <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>500</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1076</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>16</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>4</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>5.6864999999999997</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>0.18909999999999999</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>27</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>37</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>0.64100000000000001</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>7.1749999999999998</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>0.91700000000000004</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="5">
         <v>0.159</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="13">
         <v>0.86399999999999999</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="13">
         <v>0.86899999999999999</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="13">
         <v>0.86599999999999999</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="14">
         <v>0.86199999999999999</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>450</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>22054</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>98</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>1.7948</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>0.30220000000000002</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>23</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <v>44</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>0.193</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>3.2360000000000002</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="8">
         <v>0.90500000000000003</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="7"/>
+      <c r="S5" s="13">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="T5" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="V5" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>317080</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>1049866</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>13477</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>7</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>0.63200000000000001</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <v>34</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>30</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>0.69099999999999995</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="11">
         <v>6.3220000000000001</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="11">
         <v>0.85499999999999998</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
         <v>0.17299999999999999</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9">
+      <c r="S6" s="15">
+        <v>0.82</v>
+      </c>
+      <c r="T6" s="15">
         <v>0.83199999999999996</v>
       </c>
-      <c r="U6" s="9"/>
-      <c r="V6" s="10"/>
+      <c r="U6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="V6" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="I9" s="1"/>
+      <c r="I9" s="12"/>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="U10" s="5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0.53700000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated report and tabels
</commit_message>
<xml_diff>
--- a/Docs/tabels.xlsx
+++ b/Docs/tabels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\Técnico\CRC\Projeto\Workspace\CRC2021\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3830D297-CCC0-44F1-BD3D-1AB472E4E784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7769DE8E-3A5D-4A8C-ADF1-A06E88FAEDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Network</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>AT - Average Transitivity</t>
+  </si>
+  <si>
+    <t>Times (s)</t>
   </si>
 </sst>
 </file>
@@ -327,7 +330,261 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="54">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -430,134 +687,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -943,7 +1072,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31DF3AB8-3104-4D0E-8AD4-541FE248DB97}" name="Tabela1" displayName="Tabela1" ref="B2:H6" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31DF3AB8-3104-4D0E-8AD4-541FE248DB97}" name="Tabela1" displayName="Tabela1" ref="B2:H6" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
   <autoFilter ref="B2:H6" xr:uid="{31DF3AB8-3104-4D0E-8AD4-541FE248DB97}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -954,20 +1083,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BD9952FD-0516-4DE7-AC4D-017A020533D1}" name="Network" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{7386C339-71D4-47E9-BB57-576DC80A209D}" name="Nodes" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{FEEA27C9-FF81-449F-9E80-3D17946AA0B9}" name="Edges" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{4EEC6697-EC02-48E8-9668-184EE35D19F6}" name="Expected Communities" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{AEE8D59E-83A0-4523-9764-B684394C284A}" name="Average Degree" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{04D4A988-05CD-4155-AC07-A21AD8D954FB}" name="Average Path Length" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{902807E3-1B6C-4D3C-8CEC-6EB17B07CB8F}" name="Clustering Coefficient" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{BD9952FD-0516-4DE7-AC4D-017A020533D1}" name="Network" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{7386C339-71D4-47E9-BB57-576DC80A209D}" name="Nodes" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{FEEA27C9-FF81-449F-9E80-3D17946AA0B9}" name="Edges" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{4EEC6697-EC02-48E8-9668-184EE35D19F6}" name="Expected Communities" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{AEE8D59E-83A0-4523-9764-B684394C284A}" name="Average Degree" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{04D4A988-05CD-4155-AC07-A21AD8D954FB}" name="Average Path Length" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{902807E3-1B6C-4D3C-8CEC-6EB17B07CB8F}" name="Clustering Coefficient" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{599D0100-3BF9-48A2-872A-937F7ACFB5B7}" name="Tabela2" displayName="Tabela2" ref="J2:P6" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{599D0100-3BF9-48A2-872A-937F7ACFB5B7}" name="Tabela2" displayName="Tabela2" ref="J2:P6" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="J2:P6" xr:uid="{599D0100-3BF9-48A2-872A-937F7ACFB5B7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -978,20 +1107,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FD4ABEAB-CAAB-496C-BF1A-82EE5504C5A4}" name="Algorithm" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1B8DE182-6929-42F3-8465-295D7488B206}" name="Communities" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{0CD33555-C038-4D78-8C24-AF1B9E679672}" name="ACS" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{FDA597C5-604A-4969-941B-602081FA8FF7}" name="APL" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{CDA6880E-F377-42F6-8BE5-76AB5FFF22C4}" name="AID" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{4F2E73CA-E516-452D-8966-7EC0060CA68C}" name="AE" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{211C7631-7466-446F-B2F3-B8B55B460F9B}" name="AT" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{FD4ABEAB-CAAB-496C-BF1A-82EE5504C5A4}" name="Algorithm" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{1B8DE182-6929-42F3-8465-295D7488B206}" name="Communities" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{0CD33555-C038-4D78-8C24-AF1B9E679672}" name="ACS" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{FDA597C5-604A-4969-941B-602081FA8FF7}" name="APL" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{CDA6880E-F377-42F6-8BE5-76AB5FFF22C4}" name="AID" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{4F2E73CA-E516-452D-8966-7EC0060CA68C}" name="AE" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{211C7631-7466-446F-B2F3-B8B55B460F9B}" name="AT" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B536BF37-0E95-45A4-B5A0-FD1E95322902}" name="Tabela3" displayName="Tabela3" ref="R2:V6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B536BF37-0E95-45A4-B5A0-FD1E95322902}" name="Tabela3" displayName="Tabela3" ref="R2:V6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="R2:V6" xr:uid="{B536BF37-0E95-45A4-B5A0-FD1E95322902}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1000,18 +1129,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1515B093-B6CB-4BB9-864D-8655A4599932}" name="Modularity" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4DA7020B-D04E-4195-A296-D1DA38606067}" name="Louvain" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{22B2361F-79E6-4EDC-AD51-FC1AE8CE8450}" name="Leiden" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{413FC47F-EFE5-4F44-BE40-794E7E3FB01C}" name="Girvan-Newman" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{2281036E-87EA-4797-8AFC-4FE931C35092}" name="Infomap" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1515B093-B6CB-4BB9-864D-8655A4599932}" name="Modularity" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4DA7020B-D04E-4195-A296-D1DA38606067}" name="Louvain" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{22B2361F-79E6-4EDC-AD51-FC1AE8CE8450}" name="Leiden" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{413FC47F-EFE5-4F44-BE40-794E7E3FB01C}" name="Girvan-Newman" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{2281036E-87EA-4797-8AFC-4FE931C35092}" name="Infomap" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECDDCFD9-1E28-4014-B9F6-17D6A219A546}" name="Tabela4" displayName="Tabela4" ref="R9:V10" totalsRowShown="0" headerRowDxfId="5" dataDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECDDCFD9-1E28-4014-B9F6-17D6A219A546}" name="Tabela4" displayName="Tabela4" ref="R9:V10" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="R9:V10" xr:uid="{ECDDCFD9-1E28-4014-B9F6-17D6A219A546}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1020,11 +1149,31 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B01D6B58-CA1D-4487-B487-AEE57796A3A9}" name="Accuracy" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{3AF1ACE6-5EA7-409C-B81D-5FB98FF28A16}" name="Louvain" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{F77036A0-0023-4C76-9749-DD1A89774D0F}" name="Leiden" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{D6CDCBB9-D401-4A66-918B-2C2ADD1CB811}" name="Girvan-Newman" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{F6D701C3-4384-4C32-8828-AB99B57085FF}" name="Infomap" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{B01D6B58-CA1D-4487-B487-AEE57796A3A9}" name="Accuracy" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{3AF1ACE6-5EA7-409C-B81D-5FB98FF28A16}" name="Louvain" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{F77036A0-0023-4C76-9749-DD1A89774D0F}" name="Leiden" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{D6CDCBB9-D401-4A66-918B-2C2ADD1CB811}" name="Girvan-Newman" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{F6D701C3-4384-4C32-8828-AB99B57085FF}" name="Infomap" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9FBE9A14-62FC-4CEF-B87A-AC46C58C5519}" name="Tabela46" displayName="Tabela46" ref="R12:V13" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="R12:V13" xr:uid="{9FBE9A14-62FC-4CEF-B87A-AC46C58C5519}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{40C780D9-0C33-4834-95CA-B2BBE48A280B}" name="Times (s)" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A363DA6E-D0B1-45FA-8B57-4F488FFA0088}" name="Louvain" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{0AED4EBC-75D7-4020-84BF-9871EAFAC6E5}" name="Leiden" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{45146D33-A735-46D6-B8A3-276270248597}" name="Girvan-Newman" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{50BB5D0D-CBC4-4C2D-B7BA-507503D5238D}" name="Infomap" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1293,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:V12"/>
+  <dimension ref="B2:V13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,7 +1581,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="V3" s="14">
-        <v>0.36299999999999999</v>
+        <v>0.42199999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.3">
@@ -1655,7 +1804,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V10" s="6">
-        <v>0.53700000000000003</v>
+        <v>0.61609999999999998</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
@@ -1667,15 +1816,48 @@
       <c r="J12" t="s">
         <v>30</v>
       </c>
+      <c r="R12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="R13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" s="13">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="T13" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U13" s="13">
+        <v>382.82</v>
+      </c>
+      <c r="V13" s="14">
+        <v>0.26100000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final report and pdf
</commit_message>
<xml_diff>
--- a/Docs/tabels.xlsx
+++ b/Docs/tabels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\Técnico\CRC\Projeto\Workspace\CRC2021\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75863709-0A6B-448E-9CE1-06473BF1F5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37662FFF-F8E6-4A57-BBDB-E59E3B0A24AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Network</t>
   </si>
@@ -1444,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:V13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1757,8 +1757,8 @@
       <c r="U6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="16" t="s">
-        <v>24</v>
+      <c r="V6" s="16">
+        <v>0.81899999999999995</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">

</xml_diff>